<commit_message>
Analysis with Offset times
</commit_message>
<xml_diff>
--- a/Study2Analysis/Study2ValidationOnsetTimes.xlsx
+++ b/Study2Analysis/Study2ValidationOnsetTimes.xlsx
@@ -5,30 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\OneDrive - University of Glasgow\Documents\R_Scripts\Study2Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Goodge\Documents\R_Scripts\Study2Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C062144-512D-4A8B-9519-DDD6A68103E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5970DB18-DB11-4CFF-816B-1C0711E48B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -651,23 +638,23 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.15625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -722,36 +709,36 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2">
-        <v>36.144550555550495</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3">
+        <v>35.690801111108129</v>
+      </c>
+      <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>34.43</v>
       </c>
-      <c r="F3" s="2">
-        <v>1.7145505555504954</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="F3">
+        <v>1.2608011111081296</v>
+      </c>
+      <c r="G3">
         <v>15</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>62.5</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -759,7 +746,7 @@
         <v>34</v>
       </c>
       <c r="C4">
-        <v>23.67116862745268</v>
+        <v>23.942272549020373</v>
       </c>
       <c r="D4" t="s">
         <v>58</v>
@@ -768,7 +755,7 @@
         <v>22.45</v>
       </c>
       <c r="F4">
-        <v>1.2211686274526805</v>
+        <v>1.4922725490203739</v>
       </c>
       <c r="G4">
         <v>17</v>
@@ -780,7 +767,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -788,7 +775,7 @@
         <v>35</v>
       </c>
       <c r="C5">
-        <v>16.07715937503189</v>
+        <v>16.190578125019968</v>
       </c>
       <c r="D5" t="s">
         <v>59</v>
@@ -797,7 +784,7 @@
         <v>13.94</v>
       </c>
       <c r="F5">
-        <v>2.1371593750318905</v>
+        <v>2.2505781250199686</v>
       </c>
       <c r="G5">
         <v>16</v>
@@ -809,7 +796,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -838,7 +825,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -867,7 +854,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -896,7 +883,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -925,7 +912,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -954,7 +941,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -983,7 +970,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1012,7 +999,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1041,7 +1028,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1070,36 +1057,36 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="2">
-        <v>10.997349999999864</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15">
+        <v>11.455473333339334</v>
+      </c>
+      <c r="D15" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15">
         <v>9.59</v>
       </c>
-      <c r="F15" s="2">
-        <v>1.4073499999998642</v>
-      </c>
-      <c r="G15" s="2">
-        <v>12</v>
-      </c>
-      <c r="H15" s="2">
-        <v>50</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="F15">
+        <v>1.8654733333393345</v>
+      </c>
+      <c r="G15">
+        <v>15</v>
+      </c>
+      <c r="H15">
+        <v>62.5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1128,7 +1115,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1136,7 +1123,7 @@
         <v>47</v>
       </c>
       <c r="C17">
-        <v>13.664921874998647</v>
+        <v>13.711271874998895</v>
       </c>
       <c r="D17" t="s">
         <v>71</v>
@@ -1145,7 +1132,7 @@
         <v>12.78</v>
       </c>
       <c r="F17">
-        <v>0.88492187499864805</v>
+        <v>0.9312718749988953</v>
       </c>
       <c r="G17">
         <v>16</v>
@@ -1157,36 +1144,36 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>12.146846666659835</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18">
         <v>11.1</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18">
         <v>1.0468466666598353</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18">
         <v>15</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18">
         <v>62.5</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1215,7 +1202,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1244,7 +1231,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1273,7 +1260,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1281,7 +1268,7 @@
         <v>52</v>
       </c>
       <c r="C22">
-        <v>24.649836274505798</v>
+        <v>24.707594117643168</v>
       </c>
       <c r="D22" t="s">
         <v>59</v>
@@ -1290,7 +1277,7 @@
         <v>22.66</v>
       </c>
       <c r="F22">
-        <v>1.989836274505798</v>
+        <v>2.0475941176431682</v>
       </c>
       <c r="G22">
         <v>17</v>
@@ -1302,7 +1289,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1331,36 +1318,36 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="1">
-        <v>16.602179999989477</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C24" s="2">
+        <v>16.824192857164288</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="2">
         <v>15.82</v>
       </c>
-      <c r="F24" s="1">
-        <v>0.78217999998947718</v>
-      </c>
-      <c r="G24" s="1">
-        <v>10</v>
-      </c>
-      <c r="H24" s="1">
-        <v>41.666666666666671</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="F24" s="2">
+        <v>1.0041928571642877</v>
+      </c>
+      <c r="G24" s="2">
+        <v>14</v>
+      </c>
+      <c r="H24" s="2">
+        <v>58.333333333333336</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Changed summaries to exclude older/ novice and only count those who completed experiment in final numbers
</commit_message>
<xml_diff>
--- a/Study2Analysis/Study2ValidationOnsetTimes.xlsx
+++ b/Study2Analysis/Study2ValidationOnsetTimes.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Goodge\Documents\R_Scripts\Study2Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5970DB18-DB11-4CFF-816B-1C0711E48B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8741832-CF3B-4885-BC3E-82B0CEBAC6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
   <si>
     <t>ClipNumber</t>
   </si>
@@ -248,19 +261,13 @@
   </si>
   <si>
     <t>Taxi pulls into your lane</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>FALSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -275,15 +282,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,11 +293,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -310,19 +305,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -635,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="N9" sqref="N9:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +646,7 @@
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -680,65 +672,69 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2">
-        <v>23.319023076915066</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="1">
+        <v>23.192399999975351</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>22.18</v>
       </c>
-      <c r="F2" s="2">
-        <v>1.1390230769150662</v>
-      </c>
-      <c r="G2" s="2">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2">
-        <v>54.166666666666664</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F2" s="1">
+        <v>1.0123999999753508</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1">
+        <v>71.428571428571431</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>SUM(I:I)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3">
-        <v>35.690801111108129</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="1">
+        <v>35.746701388889086</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>34.43</v>
       </c>
-      <c r="F3">
-        <v>1.2608011111081296</v>
-      </c>
-      <c r="G3">
-        <v>15</v>
-      </c>
-      <c r="H3">
-        <v>62.5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <v>1.3167013888890864</v>
+      </c>
+      <c r="G3" s="1">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1">
+        <v>85.714285714285708</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -746,7 +742,7 @@
         <v>34</v>
       </c>
       <c r="C4">
-        <v>23.942272549020373</v>
+        <v>24.019052380957394</v>
       </c>
       <c r="D4" t="s">
         <v>58</v>
@@ -755,19 +751,19 @@
         <v>22.45</v>
       </c>
       <c r="F4">
-        <v>1.4922725490203739</v>
+        <v>1.5690523809573946</v>
       </c>
       <c r="G4">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H4">
-        <v>70.833333333333343</v>
-      </c>
-      <c r="I4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -775,7 +771,7 @@
         <v>35</v>
       </c>
       <c r="C5">
-        <v>16.190578125019968</v>
+        <v>16.312350000018036</v>
       </c>
       <c r="D5" t="s">
         <v>59</v>
@@ -784,48 +780,48 @@
         <v>13.94</v>
       </c>
       <c r="F5">
-        <v>2.2505781250199686</v>
+        <v>2.3723500000180362</v>
       </c>
       <c r="G5">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H5">
-        <v>66.666666666666657</v>
-      </c>
-      <c r="I5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+        <v>92.857142857142861</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="2">
-        <v>13.420910714283695</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6">
+        <v>13.358065384605876</v>
+      </c>
+      <c r="D6" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>12.42</v>
       </c>
-      <c r="F6" s="2">
-        <v>1.0009107142836946</v>
-      </c>
-      <c r="G6" s="2">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2">
-        <v>58.333333333333336</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0.93806538460587596</v>
+      </c>
+      <c r="G6">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>92.857142857142861</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -833,7 +829,7 @@
         <v>37</v>
       </c>
       <c r="C7">
-        <v>29.844341176474103</v>
+        <v>30.017392857153059</v>
       </c>
       <c r="D7" t="s">
         <v>61</v>
@@ -842,19 +838,19 @@
         <v>29.72</v>
       </c>
       <c r="F7">
-        <v>0.12434117647410403</v>
+        <v>0.29739285715305996</v>
       </c>
       <c r="G7">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H7">
-        <v>70.833333333333343</v>
-      </c>
-      <c r="I7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -862,7 +858,7 @@
         <v>38</v>
       </c>
       <c r="C8">
-        <v>35.8014411764822</v>
+        <v>35.833950000009899</v>
       </c>
       <c r="D8" t="s">
         <v>62</v>
@@ -871,19 +867,19 @@
         <v>34.909999999999997</v>
       </c>
       <c r="F8">
-        <v>0.89144117648220345</v>
+        <v>0.92395000000990279</v>
       </c>
       <c r="G8">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H8">
-        <v>70.833333333333343</v>
-      </c>
-      <c r="I8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -891,7 +887,7 @@
         <v>39</v>
       </c>
       <c r="C9">
-        <v>43.526149264712224</v>
+        <v>43.578845535719374</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
@@ -900,19 +896,19 @@
         <v>41.93</v>
       </c>
       <c r="F9">
-        <v>1.5961492647122242</v>
+        <v>1.6488455357193743</v>
       </c>
       <c r="G9">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H9">
-        <v>70.833333333333343</v>
-      </c>
-      <c r="I9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -920,7 +916,7 @@
         <v>40</v>
       </c>
       <c r="C10">
-        <v>18.044021875022974</v>
+        <v>18.064060714310102</v>
       </c>
       <c r="D10" t="s">
         <v>64</v>
@@ -929,19 +925,19 @@
         <v>16.82</v>
       </c>
       <c r="F10">
-        <v>1.2240218750229737</v>
+        <v>1.2440607143101019</v>
       </c>
       <c r="G10">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H10">
-        <v>66.666666666666657</v>
-      </c>
-      <c r="I10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -949,7 +945,7 @@
         <v>41</v>
       </c>
       <c r="C11">
-        <v>32.906397058817554</v>
+        <v>32.932667857134646</v>
       </c>
       <c r="D11" t="s">
         <v>65</v>
@@ -958,19 +954,19 @@
         <v>31.75</v>
       </c>
       <c r="F11">
-        <v>1.1563970588175536</v>
+        <v>1.1826678571346463</v>
       </c>
       <c r="G11">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H11">
-        <v>70.833333333333343</v>
-      </c>
-      <c r="I11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -978,7 +974,7 @@
         <v>42</v>
       </c>
       <c r="C12">
-        <v>23.714738235297421</v>
+        <v>23.639325000008263</v>
       </c>
       <c r="D12" t="s">
         <v>66</v>
@@ -987,19 +983,19 @@
         <v>22</v>
       </c>
       <c r="F12">
-        <v>1.7147382352974212</v>
+        <v>1.6393250000082631</v>
       </c>
       <c r="G12">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H12">
-        <v>70.833333333333343</v>
-      </c>
-      <c r="I12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1022,13 +1018,13 @@
         <v>10</v>
       </c>
       <c r="H13" s="1">
-        <v>41.666666666666671</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>71.428571428571431</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1036,7 +1032,7 @@
         <v>44</v>
       </c>
       <c r="C14">
-        <v>21.581578125012236</v>
+        <v>21.539660714299696</v>
       </c>
       <c r="D14" t="s">
         <v>68</v>
@@ -1045,19 +1041,19 @@
         <v>20.8</v>
       </c>
       <c r="F14">
-        <v>0.78157812501223489</v>
+        <v>0.7396607142996956</v>
       </c>
       <c r="G14">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H14">
-        <v>66.666666666666657</v>
-      </c>
-      <c r="I14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1065,7 +1061,7 @@
         <v>45</v>
       </c>
       <c r="C15">
-        <v>11.455473333339334</v>
+        <v>11.408061538462972</v>
       </c>
       <c r="D15" t="s">
         <v>69</v>
@@ -1074,19 +1070,19 @@
         <v>9.59</v>
       </c>
       <c r="F15">
-        <v>1.8654733333393345</v>
+        <v>1.8180615384629721</v>
       </c>
       <c r="G15">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H15">
-        <v>62.5</v>
-      </c>
-      <c r="I15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>92.857142857142861</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1094,7 +1090,7 @@
         <v>46</v>
       </c>
       <c r="C16">
-        <v>17.783017647060923</v>
+        <v>17.790678571433457</v>
       </c>
       <c r="D16" t="s">
         <v>70</v>
@@ -1103,16 +1099,16 @@
         <v>16.82</v>
       </c>
       <c r="F16">
-        <v>0.96301764706092285</v>
+        <v>0.97067857143345648</v>
       </c>
       <c r="G16">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H16">
-        <v>70.833333333333343</v>
-      </c>
-      <c r="I16" t="s">
-        <v>76</v>
+        <v>100</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1123,7 +1119,7 @@
         <v>47</v>
       </c>
       <c r="C17">
-        <v>13.711271874998895</v>
+        <v>13.70918846153549</v>
       </c>
       <c r="D17" t="s">
         <v>71</v>
@@ -1132,45 +1128,45 @@
         <v>12.78</v>
       </c>
       <c r="F17">
-        <v>0.9312718749988953</v>
+        <v>0.92918846153549062</v>
       </c>
       <c r="G17">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H17">
-        <v>66.666666666666657</v>
-      </c>
-      <c r="I17" t="s">
-        <v>76</v>
+        <v>92.857142857142861</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C18">
-        <v>12.146846666659835</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" s="1">
+        <v>12.158374999991493</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>11.1</v>
       </c>
-      <c r="F18">
-        <v>1.0468466666598353</v>
-      </c>
-      <c r="G18">
-        <v>15</v>
-      </c>
-      <c r="H18">
-        <v>62.5</v>
-      </c>
-      <c r="I18" t="s">
-        <v>76</v>
+      <c r="F18" s="1">
+        <v>1.0583749999914929</v>
+      </c>
+      <c r="G18" s="1">
+        <v>12</v>
+      </c>
+      <c r="H18" s="1">
+        <v>85.714285714285708</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1181,7 +1177,7 @@
         <v>49</v>
       </c>
       <c r="C19">
-        <v>28.887447058827217</v>
+        <v>29.0257071428606</v>
       </c>
       <c r="D19" t="s">
         <v>71</v>
@@ -1190,16 +1186,16 @@
         <v>27.91</v>
       </c>
       <c r="F19">
-        <v>0.97744705882721661</v>
+        <v>1.1157071428606002</v>
       </c>
       <c r="G19">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H19">
-        <v>70.833333333333343</v>
-      </c>
-      <c r="I19" t="s">
-        <v>76</v>
+        <v>100</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1210,7 +1206,7 @@
         <v>50</v>
       </c>
       <c r="C20">
-        <v>24.863975000008011</v>
+        <v>24.923217857149556</v>
       </c>
       <c r="D20" t="s">
         <v>72</v>
@@ -1219,16 +1215,16 @@
         <v>24.2</v>
       </c>
       <c r="F20">
-        <v>0.66397500000801202</v>
+        <v>0.72321785714955666</v>
       </c>
       <c r="G20">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H20">
-        <v>66.666666666666657</v>
-      </c>
-      <c r="I20" t="s">
-        <v>76</v>
+        <v>100</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1239,7 +1235,7 @@
         <v>51</v>
       </c>
       <c r="C21">
-        <v>9.7403588235150558</v>
+        <v>9.6714464285590793</v>
       </c>
       <c r="D21" t="s">
         <v>71</v>
@@ -1248,16 +1244,16 @@
         <v>8</v>
       </c>
       <c r="F21">
-        <v>1.7403588235150558</v>
+        <v>1.6714464285590793</v>
       </c>
       <c r="G21">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H21">
-        <v>70.833333333333343</v>
-      </c>
-      <c r="I21" t="s">
-        <v>76</v>
+        <v>100</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1268,7 +1264,7 @@
         <v>52</v>
       </c>
       <c r="C22">
-        <v>24.707594117643168</v>
+        <v>24.633492857137927</v>
       </c>
       <c r="D22" t="s">
         <v>59</v>
@@ -1277,16 +1273,16 @@
         <v>22.66</v>
       </c>
       <c r="F22">
-        <v>2.0475941176431682</v>
+        <v>1.9734928571379271</v>
       </c>
       <c r="G22">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H22">
-        <v>70.833333333333343</v>
-      </c>
-      <c r="I22" t="s">
-        <v>76</v>
+        <v>100</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1297,7 +1293,7 @@
         <v>53</v>
       </c>
       <c r="C23">
-        <v>22.687034375003726</v>
+        <v>22.754196428574833</v>
       </c>
       <c r="D23" t="s">
         <v>73</v>
@@ -1306,74 +1302,74 @@
         <v>20.72</v>
       </c>
       <c r="F23">
-        <v>1.9670343750037276</v>
+        <v>2.034196428574834</v>
       </c>
       <c r="G23">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H23">
-        <v>66.666666666666657</v>
-      </c>
-      <c r="I23" t="s">
-        <v>76</v>
+        <v>100</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="2">
-        <v>16.824192857164288</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="1">
+        <v>16.874358333355374</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>15.82</v>
       </c>
-      <c r="F24" s="2">
-        <v>1.0041928571642877</v>
-      </c>
-      <c r="G24" s="2">
-        <v>14</v>
-      </c>
-      <c r="H24" s="2">
-        <v>58.333333333333336</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>76</v>
+      <c r="F24" s="1">
+        <v>1.0543583333553741</v>
+      </c>
+      <c r="G24" s="1">
+        <v>12</v>
+      </c>
+      <c r="H24" s="1">
+        <v>85.714285714285708</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="2">
-        <v>36.698500000001715</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="1">
+        <v>36.44822000000363</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>35.479999999999997</v>
       </c>
-      <c r="F25" s="2">
-        <v>1.2185000000017183</v>
-      </c>
-      <c r="G25" s="2">
-        <v>13</v>
-      </c>
-      <c r="H25" s="2">
-        <v>54.166666666666664</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>76</v>
+      <c r="F25" s="1">
+        <v>0.96822000000363317</v>
+      </c>
+      <c r="G25" s="1">
+        <v>10</v>
+      </c>
+      <c r="H25" s="1">
+        <v>71.428571428571431</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed error that average responses rather than take the last one
</commit_message>
<xml_diff>
--- a/Study2Analysis/Study2ValidationOnsetTimes.xlsx
+++ b/Study2Analysis/Study2ValidationOnsetTimes.xlsx
@@ -5,30 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Goodge\Documents\R_Scripts\Study2Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\OneDrive - University of Glasgow\Documents\R_Scripts\Study2Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8741832-CF3B-4885-BC3E-82B0CEBAC6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFF3203-362A-43D2-8585-F62927888953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -627,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9:N10"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +633,7 @@
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -680,7 +667,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="1">
-        <v>23.192399999975351</v>
+        <v>23.053829999975051</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>56</v>
@@ -689,7 +676,7 @@
         <v>22.18</v>
       </c>
       <c r="F2" s="1">
-        <v>1.0123999999753508</v>
+        <v>0.87382999997505095</v>
       </c>
       <c r="G2" s="1">
         <v>10</v>
@@ -700,41 +687,37 @@
       <c r="I2" s="1">
         <v>0</v>
       </c>
-      <c r="K2">
-        <f>SUM(I:I)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="1">
-        <v>35.746701388889086</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3">
+        <v>35.32943333333025</v>
+      </c>
+      <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>34.43</v>
       </c>
-      <c r="F3" s="1">
-        <v>1.3167013888890864</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="F3">
+        <v>0.89943333333025066</v>
+      </c>
+      <c r="G3">
         <v>12</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3">
         <v>85.714285714285708</v>
       </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -742,7 +725,7 @@
         <v>34</v>
       </c>
       <c r="C4">
-        <v>24.019052380957394</v>
+        <v>23.54635384616234</v>
       </c>
       <c r="D4" t="s">
         <v>58</v>
@@ -751,19 +734,19 @@
         <v>22.45</v>
       </c>
       <c r="F4">
-        <v>1.5690523809573946</v>
+        <v>1.0963538461623408</v>
       </c>
       <c r="G4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4">
-        <v>100</v>
+        <v>92.857142857142861</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -771,7 +754,7 @@
         <v>35</v>
       </c>
       <c r="C5">
-        <v>16.312350000018036</v>
+        <v>16.110146153878915</v>
       </c>
       <c r="D5" t="s">
         <v>59</v>
@@ -780,7 +763,7 @@
         <v>13.94</v>
       </c>
       <c r="F5">
-        <v>2.3723500000180362</v>
+        <v>2.1701461538789157</v>
       </c>
       <c r="G5">
         <v>13</v>
@@ -792,36 +775,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6">
-        <v>13.358065384605876</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="1">
+        <v>13.743663636365817</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>12.42</v>
       </c>
-      <c r="F6">
-        <v>0.93806538460587596</v>
-      </c>
-      <c r="G6">
-        <v>13</v>
-      </c>
-      <c r="H6">
-        <v>92.857142857142861</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <v>1.3236636363658167</v>
+      </c>
+      <c r="G6" s="1">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1">
+        <v>78.571428571428569</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -829,7 +812,7 @@
         <v>37</v>
       </c>
       <c r="C7">
-        <v>30.017392857153059</v>
+        <v>29.981492307696872</v>
       </c>
       <c r="D7" t="s">
         <v>61</v>
@@ -838,19 +821,19 @@
         <v>29.72</v>
       </c>
       <c r="F7">
-        <v>0.29739285715305996</v>
+        <v>0.26149230769687293</v>
       </c>
       <c r="G7">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7">
-        <v>100</v>
+        <v>92.857142857142861</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -858,7 +841,7 @@
         <v>38</v>
       </c>
       <c r="C8">
-        <v>35.833950000009899</v>
+        <v>36.29034615386049</v>
       </c>
       <c r="D8" t="s">
         <v>62</v>
@@ -867,19 +850,19 @@
         <v>34.909999999999997</v>
       </c>
       <c r="F8">
-        <v>0.92395000000990279</v>
+        <v>1.3803461538604935</v>
       </c>
       <c r="G8">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8">
-        <v>100</v>
+        <v>92.857142857142861</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -887,7 +870,7 @@
         <v>39</v>
       </c>
       <c r="C9">
-        <v>43.578845535719374</v>
+        <v>43.283971428564392</v>
       </c>
       <c r="D9" t="s">
         <v>63</v>
@@ -896,7 +879,7 @@
         <v>41.93</v>
       </c>
       <c r="F9">
-        <v>1.6488455357193743</v>
+        <v>1.3539714285643925</v>
       </c>
       <c r="G9">
         <v>14</v>
@@ -908,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -916,7 +899,7 @@
         <v>40</v>
       </c>
       <c r="C10">
-        <v>18.064060714310102</v>
+        <v>18.003321428594113</v>
       </c>
       <c r="D10" t="s">
         <v>64</v>
@@ -925,7 +908,7 @@
         <v>16.82</v>
       </c>
       <c r="F10">
-        <v>1.2440607143101019</v>
+        <v>1.1833214285941125</v>
       </c>
       <c r="G10">
         <v>14</v>
@@ -937,7 +920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -945,7 +928,7 @@
         <v>41</v>
       </c>
       <c r="C11">
-        <v>32.932667857134646</v>
+        <v>32.869807142848934</v>
       </c>
       <c r="D11" t="s">
         <v>65</v>
@@ -954,7 +937,7 @@
         <v>31.75</v>
       </c>
       <c r="F11">
-        <v>1.1826678571346463</v>
+        <v>1.1198071428489342</v>
       </c>
       <c r="G11">
         <v>14</v>
@@ -966,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -974,7 +957,7 @@
         <v>42</v>
       </c>
       <c r="C12">
-        <v>23.639325000008263</v>
+        <v>23.600914285722499</v>
       </c>
       <c r="D12" t="s">
         <v>66</v>
@@ -983,7 +966,7 @@
         <v>22</v>
       </c>
       <c r="F12">
-        <v>1.6393250000082631</v>
+        <v>1.6009142857224994</v>
       </c>
       <c r="G12">
         <v>14</v>
@@ -995,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1003,7 +986,7 @@
         <v>43</v>
       </c>
       <c r="C13" s="1">
-        <v>26.650339999999289</v>
+        <v>26.943157142849355</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>67</v>
@@ -1012,19 +995,19 @@
         <v>26.6</v>
       </c>
       <c r="F13" s="1">
-        <v>5.0339999999287954E-2</v>
+        <v>0.34315714284935339</v>
       </c>
       <c r="G13" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H13" s="1">
-        <v>71.428571428571431</v>
+        <v>50</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1032,7 +1015,7 @@
         <v>44</v>
       </c>
       <c r="C14">
-        <v>21.539660714299696</v>
+        <v>21.497992857157271</v>
       </c>
       <c r="D14" t="s">
         <v>68</v>
@@ -1041,7 +1024,7 @@
         <v>20.8</v>
       </c>
       <c r="F14">
-        <v>0.7396607142996956</v>
+        <v>0.69799285715727066</v>
       </c>
       <c r="G14">
         <v>14</v>
@@ -1053,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1061,7 +1044,7 @@
         <v>45</v>
       </c>
       <c r="C15">
-        <v>11.408061538462972</v>
+        <v>11.176023076922972</v>
       </c>
       <c r="D15" t="s">
         <v>69</v>
@@ -1070,7 +1053,7 @@
         <v>9.59</v>
       </c>
       <c r="F15">
-        <v>1.8180615384629721</v>
+        <v>1.586023076922972</v>
       </c>
       <c r="G15">
         <v>13</v>
@@ -1082,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1119,7 +1102,7 @@
         <v>47</v>
       </c>
       <c r="C17">
-        <v>13.70918846153549</v>
+        <v>13.596830769221093</v>
       </c>
       <c r="D17" t="s">
         <v>71</v>
@@ -1128,7 +1111,7 @@
         <v>12.78</v>
       </c>
       <c r="F17">
-        <v>0.92918846153549062</v>
+        <v>0.81683076922109343</v>
       </c>
       <c r="G17">
         <v>13</v>
@@ -1141,32 +1124,32 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="1">
-        <v>12.158374999991493</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="C18">
+        <v>12.030841666658409</v>
+      </c>
+      <c r="D18" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18">
         <v>11.1</v>
       </c>
-      <c r="F18" s="1">
-        <v>1.0583749999914929</v>
-      </c>
-      <c r="G18" s="1">
+      <c r="F18">
+        <v>0.93084166665840939</v>
+      </c>
+      <c r="G18">
         <v>12</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18">
         <v>85.714285714285708</v>
       </c>
-      <c r="I18" s="1">
-        <v>0</v>
+      <c r="I18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1177,7 +1160,7 @@
         <v>49</v>
       </c>
       <c r="C19">
-        <v>29.0257071428606</v>
+        <v>29.166261538465264</v>
       </c>
       <c r="D19" t="s">
         <v>71</v>
@@ -1186,13 +1169,13 @@
         <v>27.91</v>
       </c>
       <c r="F19">
-        <v>1.1157071428606002</v>
+        <v>1.2562615384652638</v>
       </c>
       <c r="G19">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H19">
-        <v>100</v>
+        <v>92.857142857142861</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1206,7 +1189,7 @@
         <v>50</v>
       </c>
       <c r="C20">
-        <v>24.923217857149556</v>
+        <v>24.900800000001478</v>
       </c>
       <c r="D20" t="s">
         <v>72</v>
@@ -1215,7 +1198,7 @@
         <v>24.2</v>
       </c>
       <c r="F20">
-        <v>0.72321785714955666</v>
+        <v>0.70080000000147891</v>
       </c>
       <c r="G20">
         <v>14</v>
@@ -1235,7 +1218,7 @@
         <v>51</v>
       </c>
       <c r="C21">
-        <v>9.6714464285590793</v>
+        <v>9.260092857115394</v>
       </c>
       <c r="D21" t="s">
         <v>71</v>
@@ -1244,7 +1227,7 @@
         <v>8</v>
       </c>
       <c r="F21">
-        <v>1.6714464285590793</v>
+        <v>1.260092857115394</v>
       </c>
       <c r="G21">
         <v>14</v>
@@ -1264,7 +1247,7 @@
         <v>52</v>
       </c>
       <c r="C22">
-        <v>24.633492857137927</v>
+        <v>24.442507142851639</v>
       </c>
       <c r="D22" t="s">
         <v>59</v>
@@ -1273,7 +1256,7 @@
         <v>22.66</v>
       </c>
       <c r="F22">
-        <v>1.9734928571379271</v>
+        <v>1.7825071428516388</v>
       </c>
       <c r="G22">
         <v>14</v>
@@ -1293,7 +1276,7 @@
         <v>53</v>
       </c>
       <c r="C23">
-        <v>22.754196428574833</v>
+        <v>22.683685714289119</v>
       </c>
       <c r="D23" t="s">
         <v>73</v>
@@ -1302,7 +1285,7 @@
         <v>20.72</v>
       </c>
       <c r="F23">
-        <v>2.034196428574834</v>
+        <v>1.9636857142891202</v>
       </c>
       <c r="G23">
         <v>14</v>
@@ -1315,32 +1298,32 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>16.874358333355374</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24">
         <v>15.82</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24">
         <v>1.0543583333553741</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24">
         <v>12</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24">
         <v>85.714285714285708</v>
       </c>
-      <c r="I24" s="1">
-        <v>0</v>
+      <c r="I24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1351,7 +1334,7 @@
         <v>55</v>
       </c>
       <c r="C25" s="1">
-        <v>36.44822000000363</v>
+        <v>36.657511111114154</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>75</v>
@@ -1360,13 +1343,13 @@
         <v>35.479999999999997</v>
       </c>
       <c r="F25" s="1">
-        <v>0.96822000000363317</v>
+        <v>1.177511111114157</v>
       </c>
       <c r="G25" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H25" s="1">
-        <v>71.428571428571431</v>
+        <v>64.285714285714292</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>

</xml_diff>